<commit_message>
changed prox sensor for team minimouse
</commit_message>
<xml_diff>
--- a/bestellliste_merge.xlsx
+++ b/bestellliste_merge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="RS-online" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="118">
   <si>
     <t xml:space="preserve">Micromouse WS 2021/22</t>
   </si>
@@ -68,44 +68,31 @@
     <t xml:space="preserve">Team 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Proximity
-Sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">666-6568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sharp Reflektierender Sensor, 300mm, Herst. Teile-Nr.: GP2Y0A41SK0F</t>
+    <t xml:space="preserve">Motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">921-1307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faulhaber 2619 SR Bürsten-Getriebemotor DC-Getriebemotor bis 10 Ncm 1257:1, 6 V / 1,11 W, Wellen-Ø 3mm, 26 (Dia.)mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nicht lieferbar, aber Alex hat wohl noch einige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">666-8491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitaler Signalprozessor 16bit dsPIC33FJ64MC804-I/PT, 40MHz 16 KB 64 KB Flash, TQFP 44-Pin 9-Kanal x 10 Bit, 9-Kanal x</t>
   </si>
   <si>
     <t xml:space="preserve">nein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brauchen wir nicht, wenn wir die ...51... nehmen!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">921-1307</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faulhaber 2619 SR Bürsten-Getriebemotor DC-Getriebemotor bis 10 Ncm 1257:1, 6 V / 1,11 W, Wellen-Ø 3mm, 26 (Dia.)mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nicht lieferbar, aber Alex hat wohl noch einige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">666-8491</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digitaler Signalprozessor 16bit dsPIC33FJ64MC804-I/PT, 40MHz 16 KB 64 KB Flash, TQFP 44-Pin 9-Kanal x 10 Bit, 9-Kanal x</t>
   </si>
   <si>
     <t xml:space="preserve">nur einer lieferbar! Danach ab 25.04.22
@@ -113,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gesamtsumme:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summe Bestellung:</t>
   </si>
   <si>
     <t xml:space="preserve">Lieferant: Pollin</t>
@@ -205,7 +189,7 @@
     <t xml:space="preserve">71-CRCW0805J-22K </t>
   </si>
   <si>
-    <t xml:space="preserve">22 kOhm, 0805, E24: 0,131€ </t>
+    <t xml:space="preserve">22 kOhm, 0805, E24 </t>
   </si>
   <si>
     <t xml:space="preserve">71-CRCW0805J-33K</t>
@@ -370,7 +354,7 @@
     <t xml:space="preserve">426-FIT0587 </t>
   </si>
   <si>
-    <t xml:space="preserve">XT60 con</t>
+    <t xml:space="preserve">XT60 conn</t>
   </si>
   <si>
     <t xml:space="preserve">653-B3F-1002 </t>
@@ -505,7 +489,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -542,16 +526,12 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -646,14 +626,14 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="1" sqref="F22:F46 F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.71"/>
@@ -726,30 +706,30 @@
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">SUM(I7:K7)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>9.72</v>
+        <v>203.47</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">E7*D7</f>
-        <v>29.16</v>
-      </c>
-      <c r="G7" s="10" t="s">
+        <v>813.88</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -760,14 +740,14 @@
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">SUM(I8:K8)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>203.47</v>
+        <v>5.62</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">E8*D8</f>
-        <v>813.88</v>
+        <v>5.62</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>22</v>
@@ -775,77 +755,35 @@
       <c r="H8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="J8" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3"/>
+      <c r="E12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">SUM(I9:K9)</f>
-        <v>1</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>5.62</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <f aca="false">E9*D9</f>
-        <v>5.62</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F12" s="3" t="n">
+        <f aca="false">SUM(F7:F11)</f>
+        <v>819.5</v>
+      </c>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="3" t="n">
-        <f aca="false">SUM(F7:F9)</f>
-        <v>848.66</v>
-      </c>
-      <c r="H13" s="10"/>
-    </row>
-    <row r="14" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="3" t="e">
-        <f aca="false">SUM(#REF!,F9,F7)</f>
-        <v>#REF!</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-    </row>
+    <row r="17" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -856,8 +794,8 @@
     <row r="26" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -875,16 +813,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ13"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="F22:F46 A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.71"/>
@@ -899,18 +837,18 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" s="13" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" s="12" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>5</v>
@@ -919,7 +857,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>8</v>
@@ -930,38 +868,38 @@
       <c r="G6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="14" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="n">
+    <row r="7" s="13" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="n">
         <v>272136</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">SUM(H7:J7)</f>
         <v>2</v>
       </c>
-      <c r="D7" s="14" t="n">
+      <c r="D7" s="13" t="n">
         <v>13.5</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="13" t="n">
         <f aca="false">D7*C7</f>
         <v>27</v>
       </c>
       <c r="G7" s="10"/>
-      <c r="H7" s="14" t="n">
+      <c r="H7" s="13" t="n">
         <v>2</v>
       </c>
       <c r="AMI7" s="0"/>
@@ -969,7 +907,7 @@
     </row>
     <row r="8" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="n">
         <f aca="false">SUM(E7:E7)</f>
@@ -977,13 +915,8 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>0</v>
-      </c>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10"/>
@@ -991,10 +924,8 @@
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-    </row>
-    <row r="13" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" display="https://www.pollin.de"/>
@@ -1014,16 +945,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ51"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22:F46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.71"/>
@@ -1038,18 +969,18 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" s="13" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" s="12" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>5</v>
@@ -1058,7 +989,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>8</v>
@@ -1069,24 +1000,24 @@
       <c r="G6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">SUM(H7:J7)</f>
@@ -1110,10 +1041,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">SUM(H8:J8)</f>
@@ -1132,10 +1063,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">SUM(H9:J9)</f>
@@ -1154,10 +1085,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">SUM(H10:J10)</f>
@@ -1176,10 +1107,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">SUM(H11:J11)</f>
@@ -1193,10 +1124,10 @@
         <v>1.156</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>2</v>
@@ -1204,10 +1135,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">SUM(H12:J12)</f>
@@ -1226,10 +1157,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">SUM(H13:J13)</f>
@@ -1243,10 +1174,10 @@
         <v>6.34</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>2</v>
@@ -1254,10 +1185,10 @@
     </row>
     <row r="14" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">SUM(H14:J14)</f>
@@ -1271,7 +1202,7 @@
         <v>1.786</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>2</v>
@@ -1279,10 +1210,10 @@
     </row>
     <row r="15" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">SUM(H15:J15)</f>
@@ -1301,10 +1232,10 @@
     </row>
     <row r="16" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">SUM(H16:J16)</f>
@@ -1323,10 +1254,10 @@
     </row>
     <row r="17" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">SUM(H17:J17)</f>
@@ -1345,10 +1276,10 @@
     </row>
     <row r="18" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">SUM(H18:J18)</f>
@@ -1370,10 +1301,10 @@
     </row>
     <row r="19" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">SUM(H19:J19)</f>
@@ -1395,10 +1326,10 @@
     </row>
     <row r="20" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0.096</v>
@@ -1409,10 +1340,10 @@
     </row>
     <row r="21" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">SUM(H21:J21)</f>
@@ -1426,10 +1357,10 @@
         <v>58.45</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>3</v>
@@ -1440,10 +1371,10 @@
     </row>
     <row r="22" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">SUM(H22:J22)</f>
@@ -1462,10 +1393,10 @@
     </row>
     <row r="23" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">SUM(H23:J23)</f>
@@ -1487,10 +1418,10 @@
     </row>
     <row r="24" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">SUM(H24:J24)</f>
@@ -1509,10 +1440,10 @@
     </row>
     <row r="25" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">SUM(H25:J25)</f>
@@ -1531,10 +1462,10 @@
     </row>
     <row r="26" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">SUM(H26:J26)</f>
@@ -1553,10 +1484,10 @@
     </row>
     <row r="27" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">SUM(H27:J27)</f>
@@ -1575,10 +1506,10 @@
     </row>
     <row r="28" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">SUM(H28:J28)</f>
@@ -1597,10 +1528,10 @@
     </row>
     <row r="29" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">SUM(H29:J29)</f>
@@ -1622,10 +1553,10 @@
     </row>
     <row r="30" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">SUM(H30:J30)</f>
@@ -1644,10 +1575,10 @@
     </row>
     <row r="31" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">SUM(H31:J31)</f>
@@ -1666,10 +1597,10 @@
     </row>
     <row r="32" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">SUM(H32:J32)</f>
@@ -1688,10 +1619,10 @@
     </row>
     <row r="33" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">SUM(H33:J33)</f>
@@ -1710,10 +1641,10 @@
     </row>
     <row r="34" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">SUM(H34:J34)</f>
@@ -1732,10 +1663,10 @@
     </row>
     <row r="35" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(H35:J35)</f>
@@ -1749,7 +1680,7 @@
         <v>13.08</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>1</v>
@@ -1757,10 +1688,10 @@
     </row>
     <row r="36" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">SUM(H36:J36)</f>
@@ -1779,10 +1710,10 @@
     </row>
     <row r="37" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">SUM(H37:J37)</f>
@@ -1801,10 +1732,10 @@
     </row>
     <row r="38" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">SUM(H38:J38)</f>
@@ -1823,10 +1754,10 @@
     </row>
     <row r="39" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C39" s="0" t="n">
         <f aca="false">SUM(H39:J39)</f>
@@ -1845,10 +1776,10 @@
     </row>
     <row r="40" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C40" s="0" t="n">
         <f aca="false">SUM(H40:J40)</f>
@@ -1867,10 +1798,10 @@
     </row>
     <row r="41" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C41" s="0" t="n">
         <f aca="false">SUM(H41:J41)</f>
@@ -1889,10 +1820,10 @@
     </row>
     <row r="42" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C42" s="0" t="n">
         <f aca="false">SUM(H42:J42)</f>
@@ -1911,10 +1842,10 @@
     </row>
     <row r="43" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C43" s="0" t="n">
         <f aca="false">SUM(H43:J43)</f>
@@ -1933,10 +1864,10 @@
     </row>
     <row r="44" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C44" s="0" t="n">
         <f aca="false">SUM(H44:J44)</f>
@@ -1958,36 +1889,38 @@
     </row>
     <row r="45" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <f aca="false">SUM(H45:J45)</f>
+        <v>6</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>0.42</v>
       </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">D45*C45</f>
+        <v>2.52</v>
+      </c>
       <c r="H45" s="0" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D46" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E46" s="3" t="n">
-        <f aca="false">SUM(E7:E31)</f>
-        <v>138.543</v>
+        <f aca="false">SUM(E7:E45)</f>
+        <v>204.707</v>
       </c>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D47" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E47" s="3" t="n">
-        <f aca="false">SUM(E7:E12,E15:E19,E22:E31)</f>
-        <v>71.967</v>
-      </c>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10"/>
@@ -1995,10 +1928,8 @@
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10"/>
-    </row>
-    <row r="51" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -2015,16 +1946,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ13"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="F22:F46 F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.71"/>
@@ -2039,18 +1970,18 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" s="13" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" s="12" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>5</v>
@@ -2059,7 +1990,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>8</v>
@@ -2070,46 +2001,46 @@
       <c r="G6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="14" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="n">
+    <row r="7" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="n">
         <v>1420</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>121</v>
+      <c r="B7" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">SUM(H7:J7)</f>
         <v>4</v>
       </c>
-      <c r="D7" s="14" t="n">
+      <c r="D7" s="13" t="n">
         <v>4.25</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="13" t="n">
         <f aca="false">D7*C7</f>
         <v>17</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>22</v>
+      <c r="F7" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="H7" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" s="14" t="n">
+        <v>117</v>
+      </c>
+      <c r="H7" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="13" t="n">
         <v>2</v>
       </c>
       <c r="AMI7" s="0"/>
@@ -2117,7 +2048,7 @@
     </row>
     <row r="8" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="n">
         <f aca="false">SUM(E7:E7)</f>
@@ -2125,13 +2056,8 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>0</v>
-      </c>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10"/>
@@ -2139,10 +2065,8 @@
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-    </row>
-    <row r="13" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" display="https://www.pololu.com/"/>

</xml_diff>

<commit_message>
added distance sensors to mendoza bom
</commit_message>
<xml_diff>
--- a/bestellliste_merge.xlsx
+++ b/bestellliste_merge.xlsx
@@ -570,6 +570,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -762,7 +763,7 @@
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.12"/>
@@ -1127,7 +1128,7 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>
@@ -1254,10 +1255,10 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>
@@ -1680,14 +1681,14 @@
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">SUM(G22:I22)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>8.35</v>
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">D22*C22</f>
-        <v>58.45</v>
+        <v>83.5</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>87</v>
@@ -1697,6 +1698,9 @@
       </c>
       <c r="H22" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2415,7 +2419,7 @@
       </c>
       <c r="E56" s="3" t="n">
         <f aca="false">SUM(E7:E54)</f>
-        <v>223.375</v>
+        <v>248.425</v>
       </c>
       <c r="F56" s="11"/>
     </row>
@@ -2452,7 +2456,7 @@
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>

</xml_diff>

<commit_message>
diese version der bestellliste an alex versendet
</commit_message>
<xml_diff>
--- a/bestellliste_merge.xlsx
+++ b/bestellliste_merge.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="RS-online" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Pollin" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Pollin" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="RS-online" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Mouser" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Pololu" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -28,150 +28,150 @@
     <t xml:space="preserve">Micromouse WS 2021/22</t>
   </si>
   <si>
-    <t xml:space="preserve">Lieferant: RS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://de.rs-online.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bestellnummer</t>
+    <t xml:space="preserve">Lieferant: Pollin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.pollin.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bestellnr</t>
   </si>
   <si>
     <t xml:space="preserve">Beschreibung</t>
   </si>
   <si>
     <t xml:space="preserve">Menge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Einzelpreis
- (ohne Mwst)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gesamtpreis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kommentar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Team WAXN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Team minimouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mendoza et al.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">921-1307</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faulhaber 2619 SR Bürsten-Getriebemotor DC-Getriebemotor bis 10 Ncm 1257:1, 6 V / 1,11 W, Wellen-Ø 3mm, 26 (Dia.)mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nicht lieferbar, aber Alex hat wohl noch einige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">666-8491</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digitaler Signalprozessor 16bit dsPIC33FJ64MC804-I/PT, 40MHz 16 KB 64 KB Flash, TQFP 44-Pin 9-Kanal x 10 Bit, 9-Kanal x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nur einer lieferbar! Danach ab 25.04.22
-Alex hat evtl. noch welche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crystal Oscillator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">693-8819</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HC49-4H Crystal 16 MHz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inductor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">308-8570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0805 inductor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinheader 1 row</t>
-  </si>
-  <si>
-    <t xml:space="preserve">251-8632</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For programmer &amp; sensors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinheader 2x3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">832-3496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor connectors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket </t>
-  </si>
-  <si>
-    <t xml:space="preserve">488-1724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket for UART connections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H-Bridge </t>
-  </si>
-  <si>
-    <t xml:space="preserve">699-6752</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BD6222HFP-TR H-Bridge IC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voltage Regulator 3V3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">534-3021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texas Instrumens LM3940IT-3.3/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gesamtsumme:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieferant: Pollin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.pollin.de</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bestellnr</t>
   </si>
   <si>
     <t xml:space="preserve">Einzelpreis 
 (ohne Mwst)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesamtpreis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommentar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team WAXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team minimouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mendoza et al.</t>
   </si>
   <si>
     <t xml:space="preserve">
 EXTRON Modellbau-Akkupack X2, LiPo, 7,4 V-/1300 mAh, 25C
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesamtsumme:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieferant: RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://de.rs-online.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bestellnummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einzelpreis
+ (ohne Mwst)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">921-1307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faulhaber 2619 SR Bürsten-Getriebemotor DC-Getriebemotor bis 10 Ncm 1257:1, 6 V / 1,11 W, Wellen-Ø 3mm, 26 (Dia.)mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nicht lieferbar, aber Alex hat wohl noch einige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">666-8491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitaler Signalprozessor 16bit dsPIC33FJ64MC804-I/PT, 40MHz 16 KB 64 KB Flash, TQFP 44-Pin 9-Kanal x 10 Bit, 9-Kanal x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nur einer lieferbar! Danach ab 25.04.22
+Alex hat evtl. noch welche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal Oscillator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">693-8819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HC49-4H Crystal 16 MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">308-8570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805 inductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinheader 1 row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">251-8632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For programmer &amp; sensors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinheader 2x3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">832-3496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor connectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket </t>
+  </si>
+  <si>
+    <t xml:space="preserve">488-1724</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket for UART connections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-Bridge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">699-6752</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD6222HFP-TR H-Bridge IC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage Regulator 3V3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">534-3021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas Instrumens LM3940IT-3.3/</t>
   </si>
   <si>
     <t xml:space="preserve">Lieferant: Mouser</t>
@@ -551,16 +551,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <u val="single"/>
       <sz val="10"/>
+      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <i val="true"/>
       <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -614,7 +614,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -639,27 +639,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -667,11 +663,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -757,13 +757,143 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AMJ1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AMH6" s="0"/>
+      <c r="AMI6" s="0"/>
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row r="7" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="n">
+        <v>272136</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">SUM(G7:I7)</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="9" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <f aca="false">D7*C7</f>
+        <v>27</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AMH7" s="0"/>
+      <c r="AMI7" s="0"/>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <f aca="false">SUM(E7:E7)</f>
+        <v>27</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="https://www.pollin.de"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.12"/>
@@ -780,73 +910,73 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" s="12" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>13</v>
+      <c r="A7" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">SUM(H7:J7)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>203.47</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">E7*D7</f>
-        <v>813.88</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>16</v>
+        <v>1220.82</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>2</v>
@@ -854,16 +984,19 @@
       <c r="I7" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="J7" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>17</v>
+      <c r="A8" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">SUM(H8:J8)</f>
@@ -876,8 +1009,8 @@
         <f aca="false">E8*D8</f>
         <v>16.86</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>20</v>
+      <c r="G8" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>1</v>
@@ -887,14 +1020,14 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>21</v>
+      <c r="A9" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">SUM(H9:J9)</f>
@@ -907,20 +1040,20 @@
         <f aca="false">E9*D9</f>
         <v>1.3</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="10"/>
       <c r="J9" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>24</v>
+      <c r="A10" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">SUM(H10:J10)</f>
@@ -933,20 +1066,20 @@
         <f aca="false">E10*D10</f>
         <v>1.4</v>
       </c>
-      <c r="G10" s="11"/>
+      <c r="G10" s="10"/>
       <c r="J10" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>27</v>
+      <c r="A11" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">SUM(H11:J11)</f>
@@ -959,20 +1092,20 @@
         <f aca="false">E11*D11</f>
         <v>4.506</v>
       </c>
-      <c r="G11" s="11"/>
+      <c r="G11" s="10"/>
       <c r="J11" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>30</v>
+      <c r="A12" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">SUM(H12:J12)</f>
@@ -985,20 +1118,20 @@
         <f aca="false">E12*D12</f>
         <v>1.35</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="10"/>
       <c r="J12" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>33</v>
+      <c r="A13" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">SUM(H13:J13)</f>
@@ -1011,20 +1144,20 @@
         <f aca="false">E13*D13</f>
         <v>8.1</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="10"/>
       <c r="J13" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
-        <v>36</v>
+      <c r="A14" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">SUM(H14:J14)</f>
@@ -1037,20 +1170,20 @@
         <f aca="false">E14*D14</f>
         <v>14.82</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="G14" s="10"/>
       <c r="J14" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>39</v>
+      <c r="A15" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">SUM(H15:J15)</f>
@@ -1063,7 +1196,7 @@
         <f aca="false">E15*D15</f>
         <v>5.24</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="10"/>
       <c r="J15" s="0" t="n">
         <v>2</v>
       </c>
@@ -1074,13 +1207,13 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="F19" s="3" t="n">
         <f aca="false">SUM(F7:F18)</f>
-        <v>867.456</v>
-      </c>
-      <c r="G19" s="11"/>
+        <v>1274.396</v>
+      </c>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
@@ -1117,18 +1250,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>
@@ -1145,178 +1278,48 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A4" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="G6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="13" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="n">
-        <v>272136</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <f aca="false">SUM(G7:I7)</f>
-        <v>2</v>
-      </c>
-      <c r="D7" s="13" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="E7" s="13" t="n">
-        <f aca="false">D7*C7</f>
-        <v>27</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AMH7" s="0"/>
-      <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <f aca="false">SUM(E7:E7)</f>
-        <v>27</v>
-      </c>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
-    </row>
-    <row r="12" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="https://www.pollin.de"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AMH6" s="0"/>
-      <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
-    </row>
-    <row r="7" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>53</v>
       </c>
@@ -2076,7 +2079,7 @@
         <f aca="false">D39*C39</f>
         <v>13.08</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="10" t="s">
         <v>122</v>
       </c>
       <c r="G39" s="0" t="n">
@@ -2415,22 +2418,22 @@
     </row>
     <row r="56" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D56" s="3" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="E56" s="3" t="n">
         <f aca="false">SUM(E7:E54)</f>
         <v>248.425</v>
       </c>
-      <c r="F56" s="11"/>
+      <c r="F56" s="10"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="11"/>
+      <c r="A57" s="10"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="11"/>
+      <c r="A58" s="10"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="11"/>
+      <c r="A59" s="10"/>
     </row>
     <row r="60" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2456,7 +2459,7 @@
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.12"/>
@@ -2478,43 +2481,43 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="6" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+    <row r="6" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="13" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1420</v>
       </c>
@@ -2525,23 +2528,23 @@
         <f aca="false">SUM(G7:I7)</f>
         <v>3</v>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="9" t="n">
         <v>4.25</v>
       </c>
-      <c r="E7" s="13" t="n">
+      <c r="E7" s="9" t="n">
         <f aca="false">D7*C7</f>
         <v>12.75</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="13" t="n">
+      <c r="G7" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="13" t="n">
+      <c r="H7" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="13" t="n">
+      <c r="I7" s="9" t="n">
         <v>1</v>
       </c>
       <c r="AMH7" s="0"/>
@@ -2551,22 +2554,22 @@
     <row r="8" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="0"/>
       <c r="D8" s="3" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="E8" s="3" t="n">
         <f aca="false">SUM(E7:E7)</f>
         <v>12.75</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
+      <c r="A9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
+      <c r="A10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
+      <c r="A11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>